<commit_message>
- tách file excel: hoadonle, baohanh, suachua
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Tên khách hàng</t>
   </si>
@@ -94,27 +94,12 @@
     <t>Tổng tiền chi tiết (chưa CK)</t>
   </si>
   <si>
-    <t>Mã phiếu tiếp nhận</t>
-  </si>
-  <si>
-    <t>Biển số xe</t>
-  </si>
-  <si>
-    <t>Mã công ty bảo hiểm</t>
-  </si>
-  <si>
-    <t>Tên công ty bảo hiểm</t>
-  </si>
-  <si>
     <t>Tổng phải trả</t>
   </si>
   <si>
     <t>Khách đã trả</t>
   </si>
   <si>
-    <t>Bảo hiểm đã trả</t>
-  </si>
-  <si>
     <t>Tổng giảm giá</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>Tổng chi phí</t>
   </si>
   <si>
-    <t>Thu từ cọc</t>
-  </si>
-  <si>
     <t>Tiền đổi điểm</t>
   </si>
   <si>
@@ -134,24 +116,6 @@
   </si>
   <si>
     <t>Tỉnh thành</t>
-  </si>
-  <si>
-    <t>Tổng tiền BH duyệt</t>
-  </si>
-  <si>
-    <t>Khấu trừ theo vụ</t>
-  </si>
-  <si>
-    <t>BH cần trả (trước VAT)</t>
-  </si>
-  <si>
-    <t>Tổng thuế BH</t>
-  </si>
-  <si>
-    <t>BH cần trả (sau VAT)</t>
-  </si>
-  <si>
-    <t>Chế tài</t>
   </si>
 </sst>
 </file>
@@ -674,12 +638,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP33"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,37 +651,26 @@
     <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="3" max="4" width="20.5703125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="29" style="6" customWidth="1"/>
-    <col min="14" max="15" width="24.140625" style="6" customWidth="1"/>
-    <col min="16" max="16" width="27.42578125" style="17" customWidth="1"/>
-    <col min="17" max="18" width="24.42578125" style="17" customWidth="1"/>
-    <col min="19" max="20" width="18" style="17" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="17" customWidth="1"/>
-    <col min="22" max="23" width="18.140625" style="17" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" style="17" customWidth="1"/>
-    <col min="26" max="26" width="31" style="17" customWidth="1"/>
-    <col min="27" max="27" width="22" style="17" customWidth="1"/>
-    <col min="28" max="28" width="23.42578125" style="17" customWidth="1"/>
-    <col min="29" max="29" width="24.140625" style="17" customWidth="1"/>
-    <col min="30" max="30" width="22.5703125" style="17" customWidth="1"/>
-    <col min="31" max="31" width="25.7109375" style="17" customWidth="1"/>
-    <col min="32" max="38" width="19.140625" style="17" customWidth="1"/>
-    <col min="39" max="39" width="18.140625" style="17" customWidth="1"/>
-    <col min="40" max="40" width="18.140625" style="30" customWidth="1"/>
-    <col min="41" max="41" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="21.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="29" style="6" customWidth="1"/>
+    <col min="10" max="11" width="24.140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" style="17" customWidth="1"/>
+    <col min="13" max="14" width="24.42578125" style="17" customWidth="1"/>
+    <col min="15" max="16" width="18" style="17" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="17" customWidth="1"/>
+    <col min="18" max="19" width="18.140625" style="17" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="19.140625" style="17" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" style="17" customWidth="1"/>
+    <col min="28" max="28" width="18.140625" style="30" customWidth="1"/>
+    <col min="29" max="29" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
@@ -749,21 +702,9 @@
       <c r="AA1" s="34"/>
       <c r="AB1" s="34"/>
       <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD1" s="4"/>
+    </row>
+    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -775,13 +716,13 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
       <c r="S2" s="22"/>
       <c r="T2" s="22"/>
       <c r="U2" s="22"/>
@@ -791,43 +732,31 @@
       <c r="Y2" s="22"/>
       <c r="Z2" s="22"/>
       <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="26"/>
-      <c r="AO2" s="26"/>
-      <c r="AP2" s="4"/>
-    </row>
-    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="4"/>
+    </row>
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
       <c r="U3" s="22"/>
@@ -837,43 +766,31 @@
       <c r="Y3" s="22"/>
       <c r="Z3" s="22"/>
       <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="22"/>
-      <c r="AE3" s="22"/>
-      <c r="AF3" s="22"/>
-      <c r="AG3" s="22"/>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="22"/>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="22"/>
-      <c r="AL3" s="22"/>
-      <c r="AM3" s="22"/>
-      <c r="AN3" s="26"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="4"/>
-    </row>
-    <row r="4" spans="1:42" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="4"/>
+    </row>
+    <row r="4" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
       <c r="U4" s="22"/>
@@ -883,41 +800,29 @@
       <c r="Y4" s="22"/>
       <c r="Z4" s="22"/>
       <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="26"/>
-      <c r="AO4" s="26"/>
-      <c r="AP4" s="4"/>
-    </row>
-    <row r="5" spans="1:42" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="4"/>
+    </row>
+    <row r="5" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
       <c r="U5" s="22"/>
@@ -927,23 +832,11 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
       <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="22"/>
-      <c r="AI5" s="22"/>
-      <c r="AJ5" s="22"/>
-      <c r="AK5" s="22"/>
-      <c r="AL5" s="22"/>
-      <c r="AM5" s="22"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="4"/>
-    </row>
-    <row r="6" spans="1:42" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="4"/>
+    </row>
+    <row r="6" spans="1:30" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -954,136 +847,100 @@
         <v>3</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="T6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="24" t="s">
-        <v>17</v>
-      </c>
       <c r="V6" s="24" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="Y6" s="24" t="s">
         <v>30</v>
       </c>
       <c r="Z6" s="24" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="AA6" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB6" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC6" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD6" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE6" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AG6" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH6" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK6" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL6" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN6" s="7" t="s">
+      <c r="AB6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AO6" s="7" t="s">
+      <c r="AC6" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
@@ -1096,37 +953,25 @@
       <c r="Y7" s="18"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="18"/>
-      <c r="AH7" s="18"/>
-      <c r="AI7" s="18"/>
-      <c r="AJ7" s="18"/>
-      <c r="AK7" s="18"/>
-      <c r="AL7" s="18"/>
-      <c r="AM7" s="18"/>
-      <c r="AN7" s="28"/>
-      <c r="AO7" s="10"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="10"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
@@ -1139,37 +984,25 @@
       <c r="Y8" s="18"/>
       <c r="Z8" s="18"/>
       <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="18"/>
-      <c r="AI8" s="18"/>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="28"/>
-      <c r="AO8" s="10"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="10"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="10"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
@@ -1182,37 +1015,25 @@
       <c r="Y9" s="18"/>
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
-      <c r="AH9" s="18"/>
-      <c r="AI9" s="18"/>
-      <c r="AJ9" s="18"/>
-      <c r="AK9" s="18"/>
-      <c r="AL9" s="18"/>
-      <c r="AM9" s="18"/>
-      <c r="AN9" s="28"/>
-      <c r="AO9" s="10"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="10"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="10"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
@@ -1225,37 +1046,25 @@
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18"/>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="18"/>
-      <c r="AH10" s="18"/>
-      <c r="AI10" s="18"/>
-      <c r="AJ10" s="18"/>
-      <c r="AK10" s="18"/>
-      <c r="AL10" s="18"/>
-      <c r="AM10" s="18"/>
-      <c r="AN10" s="28"/>
-      <c r="AO10" s="10"/>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="10"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="10"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
@@ -1268,37 +1077,25 @@
       <c r="Y11" s="18"/>
       <c r="Z11" s="18"/>
       <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
-      <c r="AH11" s="18"/>
-      <c r="AI11" s="18"/>
-      <c r="AJ11" s="18"/>
-      <c r="AK11" s="18"/>
-      <c r="AL11" s="18"/>
-      <c r="AM11" s="18"/>
-      <c r="AN11" s="28"/>
-      <c r="AO11" s="10"/>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="10"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="10"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="18"/>
@@ -1311,37 +1108,25 @@
       <c r="Y12" s="18"/>
       <c r="Z12" s="18"/>
       <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="18"/>
-      <c r="AH12" s="18"/>
-      <c r="AI12" s="18"/>
-      <c r="AJ12" s="18"/>
-      <c r="AK12" s="18"/>
-      <c r="AL12" s="18"/>
-      <c r="AM12" s="18"/>
-      <c r="AN12" s="28"/>
-      <c r="AO12" s="10"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="10"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
@@ -1354,37 +1139,25 @@
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18"/>
-      <c r="AI13" s="18"/>
-      <c r="AJ13" s="18"/>
-      <c r="AK13" s="18"/>
-      <c r="AL13" s="18"/>
-      <c r="AM13" s="18"/>
-      <c r="AN13" s="28"/>
-      <c r="AO13" s="10"/>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="10"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="10"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="18"/>
@@ -1397,37 +1170,25 @@
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
       <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
-      <c r="AH14" s="18"/>
-      <c r="AI14" s="18"/>
-      <c r="AJ14" s="18"/>
-      <c r="AK14" s="18"/>
-      <c r="AL14" s="18"/>
-      <c r="AM14" s="18"/>
-      <c r="AN14" s="28"/>
-      <c r="AO14" s="10"/>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="10"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
@@ -1440,37 +1201,25 @@
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="18"/>
-      <c r="AH15" s="18"/>
-      <c r="AI15" s="18"/>
-      <c r="AJ15" s="18"/>
-      <c r="AK15" s="18"/>
-      <c r="AL15" s="18"/>
-      <c r="AM15" s="18"/>
-      <c r="AN15" s="28"/>
-      <c r="AO15" s="10"/>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="10"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="18"/>
@@ -1483,37 +1232,25 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="18"/>
-      <c r="AH16" s="18"/>
-      <c r="AI16" s="18"/>
-      <c r="AJ16" s="18"/>
-      <c r="AK16" s="18"/>
-      <c r="AL16" s="18"/>
-      <c r="AM16" s="18"/>
-      <c r="AN16" s="28"/>
-      <c r="AO16" s="10"/>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="10"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="18"/>
@@ -1526,37 +1263,25 @@
       <c r="Y17" s="18"/>
       <c r="Z17" s="18"/>
       <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
-      <c r="AH17" s="18"/>
-      <c r="AI17" s="18"/>
-      <c r="AJ17" s="18"/>
-      <c r="AK17" s="18"/>
-      <c r="AL17" s="18"/>
-      <c r="AM17" s="18"/>
-      <c r="AN17" s="28"/>
-      <c r="AO17" s="10"/>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="10"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="10"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
@@ -1569,37 +1294,25 @@
       <c r="Y18" s="18"/>
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
-      <c r="AJ18" s="18"/>
-      <c r="AK18" s="18"/>
-      <c r="AL18" s="18"/>
-      <c r="AM18" s="18"/>
-      <c r="AN18" s="28"/>
-      <c r="AO18" s="10"/>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="10"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="10"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="10"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="18"/>
@@ -1612,37 +1325,25 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="18"/>
       <c r="AA19" s="18"/>
-      <c r="AB19" s="18"/>
-      <c r="AC19" s="18"/>
-      <c r="AD19" s="18"/>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="18"/>
-      <c r="AG19" s="18"/>
-      <c r="AH19" s="18"/>
-      <c r="AI19" s="18"/>
-      <c r="AJ19" s="18"/>
-      <c r="AK19" s="18"/>
-      <c r="AL19" s="18"/>
-      <c r="AM19" s="18"/>
-      <c r="AN19" s="28"/>
-      <c r="AO19" s="10"/>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="10"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="10"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="10"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="18"/>
@@ -1655,37 +1356,25 @@
       <c r="Y20" s="18"/>
       <c r="Z20" s="18"/>
       <c r="AA20" s="18"/>
-      <c r="AB20" s="18"/>
-      <c r="AC20" s="18"/>
-      <c r="AD20" s="18"/>
-      <c r="AE20" s="18"/>
-      <c r="AF20" s="18"/>
-      <c r="AG20" s="18"/>
-      <c r="AH20" s="18"/>
-      <c r="AI20" s="18"/>
-      <c r="AJ20" s="18"/>
-      <c r="AK20" s="18"/>
-      <c r="AL20" s="18"/>
-      <c r="AM20" s="18"/>
-      <c r="AN20" s="28"/>
-      <c r="AO20" s="10"/>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="10"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="10"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
       <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
@@ -1698,37 +1387,25 @@
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="18"/>
-      <c r="AB21" s="18"/>
-      <c r="AC21" s="18"/>
-      <c r="AD21" s="18"/>
-      <c r="AE21" s="18"/>
-      <c r="AF21" s="18"/>
-      <c r="AG21" s="18"/>
-      <c r="AH21" s="18"/>
-      <c r="AI21" s="18"/>
-      <c r="AJ21" s="18"/>
-      <c r="AK21" s="18"/>
-      <c r="AL21" s="18"/>
-      <c r="AM21" s="18"/>
-      <c r="AN21" s="28"/>
-      <c r="AO21" s="10"/>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="10"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="10"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
       <c r="P22" s="18"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="18"/>
@@ -1741,37 +1418,25 @@
       <c r="Y22" s="18"/>
       <c r="Z22" s="18"/>
       <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="18"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="18"/>
-      <c r="AG22" s="18"/>
-      <c r="AH22" s="18"/>
-      <c r="AI22" s="18"/>
-      <c r="AJ22" s="18"/>
-      <c r="AK22" s="18"/>
-      <c r="AL22" s="18"/>
-      <c r="AM22" s="18"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="10"/>
-    </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="10"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="10"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="18"/>
@@ -1784,37 +1449,25 @@
       <c r="Y23" s="18"/>
       <c r="Z23" s="18"/>
       <c r="AA23" s="18"/>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="18"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="18"/>
-      <c r="AG23" s="18"/>
-      <c r="AH23" s="18"/>
-      <c r="AI23" s="18"/>
-      <c r="AJ23" s="18"/>
-      <c r="AK23" s="18"/>
-      <c r="AL23" s="18"/>
-      <c r="AM23" s="18"/>
-      <c r="AN23" s="28"/>
-      <c r="AO23" s="10"/>
-    </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="10"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="10"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="18"/>
@@ -1827,37 +1480,25 @@
       <c r="Y24" s="18"/>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18"/>
-      <c r="AB24" s="18"/>
-      <c r="AC24" s="18"/>
-      <c r="AD24" s="18"/>
-      <c r="AE24" s="18"/>
-      <c r="AF24" s="18"/>
-      <c r="AG24" s="18"/>
-      <c r="AH24" s="18"/>
-      <c r="AI24" s="18"/>
-      <c r="AJ24" s="18"/>
-      <c r="AK24" s="18"/>
-      <c r="AL24" s="18"/>
-      <c r="AM24" s="18"/>
-      <c r="AN24" s="28"/>
-      <c r="AO24" s="10"/>
-    </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="10"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="10"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
@@ -1870,37 +1511,25 @@
       <c r="Y25" s="18"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="18"/>
-      <c r="AB25" s="18"/>
-      <c r="AC25" s="18"/>
-      <c r="AD25" s="18"/>
-      <c r="AE25" s="18"/>
-      <c r="AF25" s="18"/>
-      <c r="AG25" s="18"/>
-      <c r="AH25" s="18"/>
-      <c r="AI25" s="18"/>
-      <c r="AJ25" s="18"/>
-      <c r="AK25" s="18"/>
-      <c r="AL25" s="18"/>
-      <c r="AM25" s="18"/>
-      <c r="AN25" s="28"/>
-      <c r="AO25" s="10"/>
-    </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="10"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
@@ -1913,37 +1542,25 @@
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
       <c r="AA26" s="18"/>
-      <c r="AB26" s="18"/>
-      <c r="AC26" s="18"/>
-      <c r="AD26" s="18"/>
-      <c r="AE26" s="18"/>
-      <c r="AF26" s="18"/>
-      <c r="AG26" s="18"/>
-      <c r="AH26" s="18"/>
-      <c r="AI26" s="18"/>
-      <c r="AJ26" s="18"/>
-      <c r="AK26" s="18"/>
-      <c r="AL26" s="18"/>
-      <c r="AM26" s="18"/>
-      <c r="AN26" s="28"/>
-      <c r="AO26" s="10"/>
-    </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="10"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
@@ -1956,37 +1573,25 @@
       <c r="Y27" s="18"/>
       <c r="Z27" s="18"/>
       <c r="AA27" s="18"/>
-      <c r="AB27" s="18"/>
-      <c r="AC27" s="18"/>
-      <c r="AD27" s="18"/>
-      <c r="AE27" s="18"/>
-      <c r="AF27" s="18"/>
-      <c r="AG27" s="18"/>
-      <c r="AH27" s="18"/>
-      <c r="AI27" s="18"/>
-      <c r="AJ27" s="18"/>
-      <c r="AK27" s="18"/>
-      <c r="AL27" s="18"/>
-      <c r="AM27" s="18"/>
-      <c r="AN27" s="28"/>
-      <c r="AO27" s="10"/>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="10"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="10"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="18"/>
@@ -1999,37 +1604,25 @@
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
-      <c r="AB28" s="18"/>
-      <c r="AC28" s="18"/>
-      <c r="AD28" s="18"/>
-      <c r="AE28" s="18"/>
-      <c r="AF28" s="18"/>
-      <c r="AG28" s="18"/>
-      <c r="AH28" s="18"/>
-      <c r="AI28" s="18"/>
-      <c r="AJ28" s="18"/>
-      <c r="AK28" s="18"/>
-      <c r="AL28" s="18"/>
-      <c r="AM28" s="18"/>
-      <c r="AN28" s="28"/>
-      <c r="AO28" s="10"/>
-    </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="10"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="10"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="18"/>
@@ -2042,37 +1635,25 @@
       <c r="Y29" s="18"/>
       <c r="Z29" s="18"/>
       <c r="AA29" s="18"/>
-      <c r="AB29" s="18"/>
-      <c r="AC29" s="18"/>
-      <c r="AD29" s="18"/>
-      <c r="AE29" s="18"/>
-      <c r="AF29" s="18"/>
-      <c r="AG29" s="18"/>
-      <c r="AH29" s="18"/>
-      <c r="AI29" s="18"/>
-      <c r="AJ29" s="18"/>
-      <c r="AK29" s="18"/>
-      <c r="AL29" s="18"/>
-      <c r="AM29" s="18"/>
-      <c r="AN29" s="28"/>
-      <c r="AO29" s="10"/>
-    </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB29" s="28"/>
+      <c r="AC29" s="10"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="10"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="18"/>
@@ -2085,22 +1666,10 @@
       <c r="Y30" s="18"/>
       <c r="Z30" s="18"/>
       <c r="AA30" s="18"/>
-      <c r="AB30" s="18"/>
-      <c r="AC30" s="18"/>
-      <c r="AD30" s="18"/>
-      <c r="AE30" s="18"/>
-      <c r="AF30" s="18"/>
-      <c r="AG30" s="18"/>
-      <c r="AH30" s="18"/>
-      <c r="AI30" s="18"/>
-      <c r="AJ30" s="18"/>
-      <c r="AK30" s="18"/>
-      <c r="AL30" s="18"/>
-      <c r="AM30" s="18"/>
-      <c r="AN30" s="28"/>
-      <c r="AO30" s="10"/>
-    </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="10"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>12</v>
       </c>
@@ -2114,32 +1683,44 @@
       <c r="I31" s="33"/>
       <c r="J31" s="33"/>
       <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="19">
+      <c r="L31" s="19">
+        <f>SUM(L$7:L30)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="19">
+        <f>SUM(M$7:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="19">
+        <f>SUM(N$7:N30)</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="25">
+        <f>SUM(O$7:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="25">
         <f>SUM(P$7:P30)</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="19">
+      <c r="Q31" s="25">
         <f>SUM(Q$7:Q30)</f>
         <v>0</v>
       </c>
-      <c r="R31" s="19">
-        <f>SUM(R$7:R30)</f>
+      <c r="R31" s="25">
+        <f xml:space="preserve"> SUM(R$7:R30)</f>
         <v>0</v>
       </c>
       <c r="S31" s="25">
-        <f>SUM(S$7:S30)</f>
+        <f xml:space="preserve"> SUM(S$7:S30)</f>
         <v>0</v>
       </c>
       <c r="T31" s="25">
-        <f>SUM(T$7:T30)</f>
+        <f xml:space="preserve"> SUM(T$7:T30)</f>
         <v>0</v>
       </c>
       <c r="U31" s="25">
-        <f>SUM(U$7:U30)</f>
+        <f xml:space="preserve"> SUM(U$7:U30)</f>
         <v>0</v>
       </c>
       <c r="V31" s="25">
@@ -2166,58 +1747,10 @@
         <f xml:space="preserve"> SUM(AA$7:AA30)</f>
         <v>0</v>
       </c>
-      <c r="AB31" s="25">
-        <f xml:space="preserve"> SUM(AB$7:AB30)</f>
-        <v>0</v>
-      </c>
-      <c r="AC31" s="25">
-        <f xml:space="preserve"> SUM(AC$7:AC30)</f>
-        <v>0</v>
-      </c>
-      <c r="AD31" s="25">
-        <f xml:space="preserve"> SUM(AD$7:AD30)</f>
-        <v>0</v>
-      </c>
-      <c r="AE31" s="25">
-        <f xml:space="preserve"> SUM(AE$7:AE30)</f>
-        <v>0</v>
-      </c>
-      <c r="AF31" s="25">
-        <f xml:space="preserve"> SUM(AF$7:AF30)</f>
-        <v>0</v>
-      </c>
-      <c r="AG31" s="25">
-        <f xml:space="preserve"> SUM(AG$7:AG30)</f>
-        <v>0</v>
-      </c>
-      <c r="AH31" s="25">
-        <f xml:space="preserve"> SUM(AH$7:AH30)</f>
-        <v>0</v>
-      </c>
-      <c r="AI31" s="25">
-        <f xml:space="preserve"> SUM(AI$7:AI30)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ31" s="25">
-        <f xml:space="preserve"> SUM(AJ$7:AJ30)</f>
-        <v>0</v>
-      </c>
-      <c r="AK31" s="25">
-        <f xml:space="preserve"> SUM(AK$7:AK30)</f>
-        <v>0</v>
-      </c>
-      <c r="AL31" s="25">
-        <f xml:space="preserve"> SUM(AL$7:AL30)</f>
-        <v>0</v>
-      </c>
-      <c r="AM31" s="25">
-        <f xml:space="preserve"> SUM(AM$7:AM30)</f>
-        <v>0</v>
-      </c>
-      <c r="AN31" s="29"/>
-      <c r="AO31" s="14"/>
-    </row>
-    <row r="33" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AB31" s="29"/>
+      <c r="AC31" s="14"/>
+    </row>
+    <row r="33" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2227,13 +1760,13 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
       <c r="S33" s="23"/>
       <c r="T33" s="23"/>
       <c r="U33" s="23"/>
@@ -2243,25 +1776,13 @@
       <c r="Y33" s="23"/>
       <c r="Z33" s="23"/>
       <c r="AA33" s="23"/>
-      <c r="AB33" s="23"/>
-      <c r="AC33" s="23"/>
-      <c r="AD33" s="23"/>
-      <c r="AE33" s="23"/>
-      <c r="AF33" s="23"/>
-      <c r="AG33" s="23"/>
-      <c r="AH33" s="23"/>
-      <c r="AI33" s="23"/>
-      <c r="AJ33" s="23"/>
-      <c r="AK33" s="23"/>
-      <c r="AL33" s="23"/>
-      <c r="AM33" s="23"/>
-      <c r="AN33" s="27"/>
-      <c r="AO33" s="27"/>
+      <c r="AB33" s="27"/>
+      <c r="AC33" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A31:O31"/>
-    <mergeCell ref="A1:AO1"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A1:AC1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>